<commit_message>
Revert "Add test to ensure an error is raised due to choice duplicates"
This reverts commit 707427ff070aa56da3316e05119c1e79cf2de0b4.
</commit_message>
<xml_diff>
--- a/onadata/apps/main/tests/fixtures/cascading_selects/new_cascading_select.xlsx
+++ b/onadata/apps/main/tests/fixtures/cascading_selects/new_cascading_select.xlsx
@@ -35,21 +35,21 @@
     <t>label</t>
   </si>
   <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
     <t>form_id</t>
   </si>
   <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>county</t>
+    <t>states</t>
   </si>
   <si>
     <t>allow_choice_duplicates</t>
   </si>
   <si>
-    <t>states</t>
-  </si>
-  <si>
     <t>texas</t>
   </si>
   <si>
@@ -65,92 +65,92 @@
     <t>counties</t>
   </si>
   <si>
+    <t>king</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>pierce</t>
+  </si>
+  <si>
+    <t>Pierce</t>
+  </si>
+  <si>
+    <t>cameron</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>cities</t>
+  </si>
+  <si>
+    <t>dumont</t>
+  </si>
+  <si>
     <t>choice_filter</t>
   </si>
   <si>
-    <t>king</t>
-  </si>
-  <si>
-    <t>King</t>
-  </si>
-  <si>
-    <t>pierce</t>
-  </si>
-  <si>
-    <t>Pierce</t>
-  </si>
-  <si>
-    <t>cameron</t>
-  </si>
-  <si>
-    <t>Cameron</t>
-  </si>
-  <si>
-    <t>cities</t>
-  </si>
-  <si>
-    <t>dumont</t>
-  </si>
-  <si>
     <t>Dumont</t>
   </si>
   <si>
+    <t>finney</t>
+  </si>
+  <si>
+    <t>Finney</t>
+  </si>
+  <si>
+    <t>brownsville</t>
+  </si>
+  <si>
+    <t>harlingen</t>
+  </si>
+  <si>
     <t>select_one states</t>
   </si>
   <si>
-    <t>finney</t>
-  </si>
-  <si>
-    <t>Finney</t>
+    <t>cascading select test</t>
+  </si>
+  <si>
+    <t>cascading_select_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True
+</t>
+  </si>
+  <si>
+    <t>seattle</t>
   </si>
   <si>
     <t>select_one counties</t>
   </si>
   <si>
-    <t>cascading select test</t>
-  </si>
-  <si>
-    <t>cascading_select_test</t>
-  </si>
-  <si>
-    <t>brownsville</t>
+    <t>Seattle</t>
   </si>
   <si>
     <t>state=${state}</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes
-</t>
+    <t>redmond</t>
+  </si>
+  <si>
+    <t>Redmond</t>
   </si>
   <si>
     <t>select_one cities</t>
   </si>
   <si>
+    <t>tacoma</t>
+  </si>
+  <si>
     <t>city</t>
   </si>
   <si>
-    <t>harlingen</t>
+    <t>Tacoma</t>
   </si>
   <si>
     <t>state=${state} and county=${county}</t>
-  </si>
-  <si>
-    <t>seattle</t>
-  </si>
-  <si>
-    <t>Seattle</t>
-  </si>
-  <si>
-    <t>redmond</t>
-  </si>
-  <si>
-    <t>Redmond</t>
-  </si>
-  <si>
-    <t>tacoma</t>
-  </si>
-  <si>
-    <t>Tacoma</t>
   </si>
   <si>
     <t>puyallup</t>
@@ -455,7 +455,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="1"/>
@@ -476,41 +476,41 @@
     </row>
     <row r="2" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" ht="16.5" customHeight="1"/>
@@ -1550,15 +1550,15 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
@@ -1583,10 +1583,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -1597,10 +1597,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
@@ -1611,10 +1611,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -1625,10 +1625,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
@@ -1636,10 +1636,10 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>24</v>
@@ -1648,114 +1648,114 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>44</v>
@@ -1767,7 +1767,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1"/>
@@ -2787,23 +2787,23 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>

</xml_diff>